<commit_message>
Final Report Changes 1
</commit_message>
<xml_diff>
--- a/docs/Images/BOM.xlsx
+++ b/docs/Images/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mittl\Desktop\ASU\ASU 2025\Spring 2025\EGR314\Github Website\E-Mittl.github.io\docs\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2E871-DF2B-4C7D-9F96-D7362CD040B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247189CC-1FAE-4D91-88EE-F9ED9DAE7DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{CE54E565-8C02-48F6-8AE4-5BBB8D22CD20}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
   <si>
     <t>Part Name</t>
   </si>
@@ -101,21 +101,12 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>PIC18F27Q84-E/5N</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/microchip-technology/PIC18F27Q84-E-5N/13691137</t>
-  </si>
-  <si>
     <t>https://ww1.microchip.com/downloads/aemDocuments/documents/MCU08/ProductDocuments/DataSheets/PIC18F27-47-57Q84-Data-Sheet-40002213E.pdf</t>
   </si>
   <si>
     <t>Digikey</t>
   </si>
   <si>
-    <t>150-PIC18F27Q84-E/5N-ND</t>
-  </si>
-  <si>
     <t>TI OPT4060</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>https://www.ti.com/lit/ds/symlink/opt4060.pdf?ts=1704223000280</t>
   </si>
   <si>
-    <t>296-OPT4060DTSRCT-ND</t>
-  </si>
-  <si>
     <t>L6981C33DR</t>
   </si>
   <si>
@@ -164,21 +152,6 @@
     <t>Illumination LED</t>
   </si>
   <si>
-    <t>Cree LED</t>
-  </si>
-  <si>
-    <t>JB2835BWT-G-U40EA0000-N000P001</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/cree-JB2835BWT-G-U40EA0000-N000P001/21531775</t>
-  </si>
-  <si>
-    <t>https://downloads.cree-led.com/files/ds/j/JSeries-2835-Pro9.pdf</t>
-  </si>
-  <si>
-    <t>2138-JB2835BWT-G-U40EA0000-N000P001CT-ND</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -371,21 +344,9 @@
     <t>R4</t>
   </si>
   <si>
-    <t>15 Ohm Resistor</t>
-  </si>
-  <si>
     <t>Illumination LED Resistor</t>
   </si>
   <si>
-    <t>RMCF0805FT15R0</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT15R0/1760514</t>
-  </si>
-  <si>
-    <t>RMCF0805FT15R0CT-ND</t>
-  </si>
-  <si>
     <t>FDV303N</t>
   </si>
   <si>
@@ -413,87 +374,12 @@
     <t>Wall Adapter Barrel Jack</t>
   </si>
   <si>
-    <t>Same Sky</t>
-  </si>
-  <si>
-    <t>PJ-006A-SMT-TR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/same-sky-formerly-cui-devices/PJ-006A-SMT-TR/408456</t>
-  </si>
-  <si>
-    <t>https://www.sameskydevices.com/product/resource/pj-006a-smt.pdf</t>
-  </si>
-  <si>
-    <t>CP-006APJCT-ND</t>
-  </si>
-  <si>
-    <t>2x4 Male Header</t>
-  </si>
-  <si>
-    <t>UART Headers</t>
-  </si>
-  <si>
-    <t>Würth Elektronik</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/61200821621/4846916</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/61200821621.pdf</t>
-  </si>
-  <si>
-    <t>732-5395-ND</t>
-  </si>
-  <si>
     <t>J2,J3</t>
   </si>
   <si>
-    <t>General Jumper Pins</t>
-  </si>
-  <si>
-    <t>2 x20 Male Header Pins</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx21121.pdf</t>
-  </si>
-  <si>
-    <t>732-5310-ND</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>J5,J6,J7,J8,J9,J11,J12</t>
-  </si>
-  <si>
-    <t>Jumper</t>
-  </si>
-  <si>
-    <t>General Purpose Jumpers</t>
-  </si>
-  <si>
-    <t>Sullins Connector Solutions</t>
-  </si>
-  <si>
-    <t>QPC02SXGN-RC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262</t>
-  </si>
-  <si>
-    <t>https://s3.amazonaws.com/catalogspreads-pdf/PAGE128-129%20.100%20JUMPER.pdf</t>
-  </si>
-  <si>
-    <t>S9337-ND</t>
-  </si>
-  <si>
-    <t>J5,J6,J7,J8,J9,J11,J13</t>
-  </si>
-  <si>
     <t>Test Points</t>
   </si>
   <si>
@@ -564,6 +450,84 @@
   </si>
   <si>
     <t>1276-1871-1-ND</t>
+  </si>
+  <si>
+    <t>TI OPT4048</t>
+  </si>
+  <si>
+    <t>296-OPT4048DTSRCT-ND</t>
+  </si>
+  <si>
+    <t>Samsung Semiconductor, Inc.</t>
+  </si>
+  <si>
+    <t>SPMWHT541MP5WAR0S5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-semiconductor-inc/SPMWHT541MP5WAR0S5/5959262</t>
+  </si>
+  <si>
+    <t>https://download.led.samsung.com/led/file/resource/2022/05/Data_Sheet_LM561B_Plus_CRI80_Rev.9.2.pdf</t>
+  </si>
+  <si>
+    <t>1510-1519-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/pic18f27q84-i-so/12807406</t>
+  </si>
+  <si>
+    <t>150-PIC18F27Q84-I/S)-ND</t>
+  </si>
+  <si>
+    <t>PIC18F27Q84-I/SO</t>
+  </si>
+  <si>
+    <t>Tensility International Corp</t>
+  </si>
+  <si>
+    <t>54-00165</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/54-00165/10459297</t>
+  </si>
+  <si>
+    <t>https://tensility.s3.us-west-2.amazonaws.com/uploads/pdffiles/54-00165.pdf</t>
+  </si>
+  <si>
+    <t>839-54-00165CT-ND</t>
+  </si>
+  <si>
+    <t>Pushbutton</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>Debugging pushbutton</t>
+  </si>
+  <si>
+    <t>PTS526SK15SMTR2 LFS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/PTS526SK15SMTR2-LFS/10056626</t>
+  </si>
+  <si>
+    <t>https://www.ckswitches.com/media/2780/pts526.pdf</t>
+  </si>
+  <si>
+    <t>CKN12221-1-ND</t>
+  </si>
+  <si>
+    <t>5.1 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0805FT5R10</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT5R10/1713185</t>
+  </si>
+  <si>
+    <t>RMCF0805FT5R10CT-ND</t>
   </si>
 </sst>
 </file>
@@ -617,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -631,6 +595,10 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -973,7 +941,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -985,7 +953,7 @@
     <col min="5" max="5" width="15.26171875" customWidth="1"/>
     <col min="6" max="6" width="19.41796875" customWidth="1"/>
     <col min="7" max="7" width="19.9453125" customWidth="1"/>
-    <col min="8" max="8" width="21.05078125" customWidth="1"/>
+    <col min="8" max="8" width="24.26171875" customWidth="1"/>
     <col min="9" max="9" width="24.3671875" customWidth="1"/>
     <col min="10" max="10" width="12.9453125" customWidth="1"/>
     <col min="11" max="11" width="13.578125" customWidth="1"/>
@@ -1057,38 +1025,39 @@
         <v>19</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>2.0299999999999998</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3">
         <f>C2*D2</f>
-        <v>10.149999999999999</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3">
-        <v>1.88</v>
+        <v>1.66</v>
       </c>
       <c r="G2" s="3">
-        <v>1.88</v>
+        <f>F2*C2</f>
+        <v>1.66</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="N2" s="2">
         <v>5</v>
@@ -1104,44 +1073,45 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>2.88</v>
+        <v>1.81</v>
       </c>
       <c r="E3" s="3">
         <f>C3*D3</f>
-        <v>11.52</v>
+        <v>1.81</v>
       </c>
       <c r="F3" s="3">
-        <v>0.88</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="G3" s="3">
-        <v>0.88</v>
+        <f t="shared" ref="G3:G19" si="0">F3*C3</f>
+        <v>1.1579999999999999</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="N3" s="2">
         <v>5</v>
@@ -1152,49 +1122,50 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3">
         <v>2.8</v>
       </c>
       <c r="E4" s="3">
         <f>C4*D4</f>
-        <v>8.3999999999999986</v>
+        <v>2.8</v>
       </c>
       <c r="F4" s="3">
         <v>1.22</v>
       </c>
       <c r="G4" s="3">
+        <f t="shared" si="0"/>
         <v>1.22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N4" s="2">
         <v>5</v>
@@ -1205,49 +1176,50 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
         <v>0.35</v>
       </c>
       <c r="E5" s="3">
         <f>C5*D5</f>
-        <v>1.75</v>
+        <v>0.35</v>
       </c>
       <c r="F5" s="3">
         <v>0.14399999999999999</v>
       </c>
       <c r="G5" s="3">
+        <f t="shared" si="0"/>
         <v>0.14399999999999999</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="N5" s="2">
         <v>10</v>
@@ -1258,49 +1230,50 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E6" s="3">
         <f>C6*D6</f>
-        <v>0.12</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F6" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G6" s="3">
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.2E-2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="N6" s="2">
         <v>20</v>
@@ -1311,49 +1284,50 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E9" si="0">C7*D7</f>
-        <v>0.08</v>
+        <f t="shared" ref="E7:E9" si="1">C7*D7</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F7" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G7" s="3">
+        <f t="shared" si="0"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="N7" s="2">
         <v>10</v>
@@ -1364,49 +1338,50 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <v>0.05</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.05</v>
       </c>
       <c r="F8" s="3">
         <v>1.4E-2</v>
       </c>
       <c r="G8" s="3">
+        <f t="shared" si="0"/>
         <v>1.4E-2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="N8" s="2">
         <v>10</v>
@@ -1417,49 +1392,50 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
+        <f t="shared" si="1"/>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="F9" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="G9" s="3">
+        <f t="shared" si="0"/>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="N9" s="2">
         <v>10</v>
@@ -1470,52 +1446,53 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ref="E10:E23" si="1">C10*D10</f>
-        <v>2.4</v>
+        <f t="shared" ref="E10:E19" si="2">C10*D10</f>
+        <v>0.2</v>
       </c>
       <c r="F10" s="3">
         <v>0.06</v>
       </c>
       <c r="G10" s="3">
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
       <c r="N10" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O10" s="5">
         <v>45716</v>
@@ -1523,49 +1500,50 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
         <v>0.125</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f t="shared" si="2"/>
+        <v>0.125</v>
       </c>
       <c r="F11" s="3">
-        <v>0.04</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="G11" s="3">
-        <v>0.04</v>
+        <f t="shared" si="0"/>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="N11" s="2">
         <v>20</v>
@@ -1576,49 +1554,50 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <v>0.125</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f t="shared" si="2"/>
+        <v>0.125</v>
       </c>
       <c r="F12" s="3">
         <v>0.125</v>
       </c>
       <c r="G12" s="3">
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="N12" s="2">
         <v>20</v>
@@ -1629,49 +1608,50 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
         <v>0.158</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>0.79</v>
+        <f t="shared" si="2"/>
+        <v>0.158</v>
       </c>
       <c r="F13" s="3">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="G13" s="3">
+        <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="N13" s="2">
         <v>5</v>
@@ -1682,49 +1662,50 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
         <v>0.192</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.96</v>
+        <f t="shared" si="2"/>
+        <v>0.192</v>
       </c>
       <c r="F14" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="G14" s="3">
+        <f t="shared" si="0"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N14" s="2">
         <v>5</v>
@@ -1735,50 +1716,50 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>1.25</v>
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F15" s="3">
         <v>2E-3</v>
       </c>
       <c r="G15" s="3">
-        <f>0.002*6</f>
-        <v>1.2E-2</v>
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="N15" s="2">
         <v>50</v>
@@ -1789,49 +1770,50 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F16" s="3">
         <v>2E-3</v>
       </c>
       <c r="G16" s="3">
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="K16" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="N16" s="2">
         <v>10</v>
@@ -1842,49 +1824,50 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C17" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>0.03</v>
       </c>
       <c r="F17" s="3">
-        <v>2E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G17" s="3">
-        <v>2E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="N17" s="2">
         <v>10</v>
@@ -1895,50 +1878,50 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D18" s="3">
         <v>0.20699999999999999</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0699999999999998</v>
+        <f t="shared" si="2"/>
+        <v>0.621</v>
       </c>
       <c r="F18" s="3">
         <v>4.6300000000000001E-2</v>
       </c>
       <c r="G18" s="3">
-        <f>F18*3</f>
+        <f t="shared" si="0"/>
         <v>0.1389</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="N18" s="2">
         <v>10</v>
@@ -1949,49 +1932,50 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
-        <v>0.95</v>
+        <v>0.89</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
+        <f t="shared" si="2"/>
+        <v>0.89</v>
       </c>
       <c r="F19" s="3">
-        <v>0.44600000000000001</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="G19" s="3">
-        <v>0.44600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.67500000000000004</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="N19" s="2">
         <v>3</v>
@@ -2002,53 +1986,53 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C20" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D20" s="3">
-        <v>0.97</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="1"/>
-        <v>2.91</v>
+        <f>C20*D20</f>
+        <v>2.0960000000000001</v>
       </c>
       <c r="F20" s="3">
-        <v>0.51300000000000001</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="G20" s="3">
-        <f>F20*2</f>
-        <v>1.026</v>
+        <f>F20*C20</f>
+        <v>1.1439999999999999</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="I20" s="2">
-        <v>61200821621</v>
+        <v>5006</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="N20" s="2">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="O20" s="5">
         <v>45716</v>
@@ -2056,167 +2040,82 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>1.81</v>
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.127</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="1"/>
-        <v>3.62</v>
+        <f>C21*D21</f>
+        <v>0.127</v>
       </c>
       <c r="F21" s="3">
-        <v>0.88600000000000001</v>
+        <v>8.8700000000000001E-2</v>
       </c>
       <c r="G21" s="3">
-        <v>0.88600000000000001</v>
+        <f>F21*C21</f>
+        <v>8.8700000000000001E-2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I21" s="2">
-        <v>61304021121</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>140</v>
+        <v>154</v>
+      </c>
+      <c r="I21" t="s">
+        <v>156</v>
+      </c>
+      <c r="J21" t="s">
+        <v>157</v>
+      </c>
+      <c r="K21" t="s">
+        <v>158</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="5">
+        <v>22</v>
+      </c>
+      <c r="M21" t="s">
+        <v>159</v>
+      </c>
+      <c r="N21" s="2">
+        <v>10</v>
+      </c>
+      <c r="O21" s="6">
         <v>45716</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="2">
-        <v>50</v>
-      </c>
-      <c r="D22" s="3">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="1"/>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G22" s="3">
-        <f>F22*10</f>
-        <v>0.25</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="N22" s="2">
-        <v>50</v>
-      </c>
-      <c r="O22" s="5">
-        <v>45716</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="5"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="2">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="1"/>
-        <v>2.62</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G23" s="3">
-        <f>F23*7</f>
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I23" s="2">
-        <v>5006</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="N23" s="2">
-        <v>25</v>
-      </c>
-      <c r="O23" s="5">
-        <v>45716</v>
-      </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="R22" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" s="1"/>
@@ -2272,29 +2171,22 @@
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{3F5D68B8-1A0F-4C75-9549-4E3CC6AD5EEB}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{51622C1D-F943-4CAA-B2AA-81C7BE8E9245}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{E001B2A2-3682-4D1C-A1B8-6B1019C2BBBA}"/>
-    <hyperlink ref="J6" r:id="rId4" xr:uid="{948EA757-C160-44C7-B828-FE5F0CB4F87F}"/>
-    <hyperlink ref="J15" r:id="rId5" xr:uid="{EA63FDE1-86E2-49E8-8FDB-6A39B624532D}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{25220359-1CF9-4713-B887-F7DB62E93025}"/>
-    <hyperlink ref="J7" r:id="rId7" xr:uid="{C9381CEB-D604-4398-8088-A7FC8F4D7D72}"/>
-    <hyperlink ref="J8" r:id="rId8" xr:uid="{334F0833-1E6D-47D1-85A3-F9554A819627}"/>
-    <hyperlink ref="J9" r:id="rId9" xr:uid="{F42F3B9D-780C-455A-8D90-71C0B46F9334}"/>
-    <hyperlink ref="J10" r:id="rId10" xr:uid="{3F66FBF7-E9FE-4DC7-A998-186DA32B3471}"/>
-    <hyperlink ref="J11" r:id="rId11" xr:uid="{BFA67FED-3ED2-41CA-BA63-43AA2C6E81E3}"/>
-    <hyperlink ref="J12" r:id="rId12" xr:uid="{CAD23BBB-F465-4DBB-BFBD-6D80440384A4}"/>
-    <hyperlink ref="J13" r:id="rId13" xr:uid="{CFBECA80-DB53-4EC9-A0D3-96FE5A624148}"/>
-    <hyperlink ref="J14" r:id="rId14" xr:uid="{FA9CA7BA-EAAB-4C70-A8EE-A7B3370F0CDF}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{C93DFBD9-00C0-4D46-AAF5-6C46883AE940}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{83CEC5D8-8DCC-494F-9885-38C0FC829101}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{5972E0C6-5A22-4762-BC6B-298C4DA10819}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{94E094FC-3690-477D-BCD5-DB7E60EC2193}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{EA25C5FE-E0F8-4222-9031-7D3C9FD0322B}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{C9CD15C6-8A50-4E74-A3A5-9D7AC5811DCA}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{566288AA-275D-4B95-AB5D-6438C590A84A}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{0EC7E269-510E-475E-BFD1-FD1483C36B6B}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{948EA757-C160-44C7-B828-FE5F0CB4F87F}"/>
+    <hyperlink ref="J15" r:id="rId4" xr:uid="{EA63FDE1-86E2-49E8-8FDB-6A39B624532D}"/>
+    <hyperlink ref="J3" r:id="rId5" xr:uid="{25220359-1CF9-4713-B887-F7DB62E93025}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{C9381CEB-D604-4398-8088-A7FC8F4D7D72}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{334F0833-1E6D-47D1-85A3-F9554A819627}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{F42F3B9D-780C-455A-8D90-71C0B46F9334}"/>
+    <hyperlink ref="J11" r:id="rId9" xr:uid="{BFA67FED-3ED2-41CA-BA63-43AA2C6E81E3}"/>
+    <hyperlink ref="J12" r:id="rId10" xr:uid="{CAD23BBB-F465-4DBB-BFBD-6D80440384A4}"/>
+    <hyperlink ref="J13" r:id="rId11" xr:uid="{CFBECA80-DB53-4EC9-A0D3-96FE5A624148}"/>
+    <hyperlink ref="J14" r:id="rId12" xr:uid="{FA9CA7BA-EAAB-4C70-A8EE-A7B3370F0CDF}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{C93DFBD9-00C0-4D46-AAF5-6C46883AE940}"/>
+    <hyperlink ref="J18" r:id="rId14" xr:uid="{5972E0C6-5A22-4762-BC6B-298C4DA10819}"/>
+    <hyperlink ref="J20" r:id="rId15" xr:uid="{0EC7E269-510E-475E-BFD1-FD1483C36B6B}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="39" orientation="landscape" r:id="rId23"/>
+  <pageSetup scale="38" orientation="landscape" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>